<commit_message>
adding column data more data
</commit_message>
<xml_diff>
--- a/Comedores_comunitarios_de_Santiago_de_Cali_a_trav_s_de_TIO.xlsx
+++ b/Comedores_comunitarios_de_Santiago_de_Cali_a_trav_s_de_TIO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="932">
   <si>
     <t>row ID</t>
   </si>
@@ -2812,6 +2812,9 @@
   </si>
   <si>
     <t>data</t>
+  </si>
+  <si>
+    <t>add</t>
   </si>
 </sst>
 </file>
@@ -3129,15 +3132,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K147"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K147"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3171,8 +3174,11 @@
       <c r="K1" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3206,8 +3212,11 @@
       <c r="K2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -3241,8 +3250,11 @@
       <c r="K3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3276,8 +3288,11 @@
       <c r="K4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -3311,8 +3326,11 @@
       <c r="K5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -3343,8 +3361,11 @@
       <c r="K6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -3375,8 +3396,11 @@
       <c r="K7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -3410,8 +3434,11 @@
       <c r="K8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -3445,8 +3472,11 @@
       <c r="K9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -3480,8 +3510,11 @@
       <c r="K10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -3515,8 +3548,11 @@
       <c r="K11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -3550,8 +3586,11 @@
       <c r="K12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -3585,8 +3624,11 @@
       <c r="K13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -3620,8 +3662,11 @@
       <c r="K14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -3655,8 +3700,11 @@
       <c r="K15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -3690,8 +3738,11 @@
       <c r="K16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -3725,8 +3776,11 @@
       <c r="K17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -3760,8 +3814,11 @@
       <c r="K18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -3795,8 +3852,11 @@
       <c r="K19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>128</v>
       </c>
@@ -3830,8 +3890,11 @@
       <c r="K20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>135</v>
       </c>
@@ -3865,8 +3928,11 @@
       <c r="K21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>141</v>
       </c>
@@ -3900,8 +3966,11 @@
       <c r="K22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -3935,8 +4004,11 @@
       <c r="K23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>153</v>
       </c>
@@ -3970,8 +4042,11 @@
       <c r="K24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>160</v>
       </c>
@@ -4005,8 +4080,11 @@
       <c r="K25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>167</v>
       </c>
@@ -4040,8 +4118,11 @@
       <c r="K26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>173</v>
       </c>
@@ -4075,8 +4156,11 @@
       <c r="K27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>179</v>
       </c>
@@ -4110,8 +4194,11 @@
       <c r="K28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>182</v>
       </c>
@@ -4145,8 +4232,11 @@
       <c r="K29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>189</v>
       </c>
@@ -4180,8 +4270,11 @@
       <c r="K30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>195</v>
       </c>
@@ -4215,8 +4308,11 @@
       <c r="K31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>201</v>
       </c>
@@ -4250,8 +4346,11 @@
       <c r="K32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>207</v>
       </c>
@@ -4285,8 +4384,11 @@
       <c r="K33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>214</v>
       </c>
@@ -4320,8 +4422,11 @@
       <c r="K34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>221</v>
       </c>
@@ -4355,8 +4460,11 @@
       <c r="K35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>228</v>
       </c>
@@ -4390,8 +4498,11 @@
       <c r="K36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>235</v>
       </c>
@@ -4425,8 +4536,11 @@
       <c r="K37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>242</v>
       </c>
@@ -4460,8 +4574,11 @@
       <c r="K38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>248</v>
       </c>
@@ -4495,8 +4612,11 @@
       <c r="K39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>254</v>
       </c>
@@ -4530,8 +4650,11 @@
       <c r="K40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>261</v>
       </c>
@@ -4565,8 +4688,11 @@
       <c r="K41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>268</v>
       </c>
@@ -4600,8 +4726,11 @@
       <c r="K42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>274</v>
       </c>
@@ -4635,8 +4764,11 @@
       <c r="K43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>281</v>
       </c>
@@ -4670,8 +4802,11 @@
       <c r="K44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>288</v>
       </c>
@@ -4705,8 +4840,11 @@
       <c r="K45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>295</v>
       </c>
@@ -4740,8 +4878,11 @@
       <c r="K46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L46">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>300</v>
       </c>
@@ -4775,8 +4916,11 @@
       <c r="K47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L47">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>306</v>
       </c>
@@ -4810,8 +4954,11 @@
       <c r="K48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>313</v>
       </c>
@@ -4845,8 +4992,11 @@
       <c r="K49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>320</v>
       </c>
@@ -4880,8 +5030,11 @@
       <c r="K50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>327</v>
       </c>
@@ -4915,8 +5068,11 @@
       <c r="K51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>333</v>
       </c>
@@ -4950,8 +5106,11 @@
       <c r="K52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>340</v>
       </c>
@@ -4985,8 +5144,11 @@
       <c r="K53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L53">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>346</v>
       </c>
@@ -5020,8 +5182,11 @@
       <c r="K54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>353</v>
       </c>
@@ -5055,8 +5220,11 @@
       <c r="K55">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>360</v>
       </c>
@@ -5090,8 +5258,11 @@
       <c r="K56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>365</v>
       </c>
@@ -5125,8 +5296,11 @@
       <c r="K57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>371</v>
       </c>
@@ -5160,8 +5334,11 @@
       <c r="K58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>378</v>
       </c>
@@ -5195,8 +5372,11 @@
       <c r="K59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>384</v>
       </c>
@@ -5230,8 +5410,11 @@
       <c r="K60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>391</v>
       </c>
@@ -5265,8 +5448,11 @@
       <c r="K61">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>397</v>
       </c>
@@ -5300,8 +5486,11 @@
       <c r="K62">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>403</v>
       </c>
@@ -5335,8 +5524,11 @@
       <c r="K63">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L63">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>409</v>
       </c>
@@ -5370,8 +5562,11 @@
       <c r="K64">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L64">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>414</v>
       </c>
@@ -5405,8 +5600,11 @@
       <c r="K65">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L65">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>419</v>
       </c>
@@ -5440,8 +5638,11 @@
       <c r="K66">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>424</v>
       </c>
@@ -5475,8 +5676,11 @@
       <c r="K67">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L67">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>431</v>
       </c>
@@ -5510,8 +5714,11 @@
       <c r="K68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L68">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>436</v>
       </c>
@@ -5545,8 +5752,11 @@
       <c r="K69">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L69">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>442</v>
       </c>
@@ -5580,8 +5790,11 @@
       <c r="K70">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L70">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>448</v>
       </c>
@@ -5615,8 +5828,11 @@
       <c r="K71">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L71">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>454</v>
       </c>
@@ -5650,8 +5866,11 @@
       <c r="K72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L72">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>461</v>
       </c>
@@ -5685,8 +5904,11 @@
       <c r="K73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L73">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>468</v>
       </c>
@@ -5720,8 +5942,11 @@
       <c r="K74">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L74">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>474</v>
       </c>
@@ -5755,8 +5980,11 @@
       <c r="K75">
         <v>5</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L75">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>481</v>
       </c>
@@ -5790,8 +6018,11 @@
       <c r="K76">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L76">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>486</v>
       </c>
@@ -5825,8 +6056,11 @@
       <c r="K77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L77">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>493</v>
       </c>
@@ -5860,8 +6094,11 @@
       <c r="K78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L78">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>499</v>
       </c>
@@ -5895,8 +6132,11 @@
       <c r="K79">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L79">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>505</v>
       </c>
@@ -5930,8 +6170,11 @@
       <c r="K80">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L80">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>511</v>
       </c>
@@ -5965,8 +6208,11 @@
       <c r="K81">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L81">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>518</v>
       </c>
@@ -6000,8 +6246,11 @@
       <c r="K82">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L82">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>524</v>
       </c>
@@ -6035,8 +6284,11 @@
       <c r="K83">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L83">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>530</v>
       </c>
@@ -6070,8 +6322,11 @@
       <c r="K84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L84">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>537</v>
       </c>
@@ -6105,8 +6360,11 @@
       <c r="K85">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L85">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>544</v>
       </c>
@@ -6140,8 +6398,11 @@
       <c r="K86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L86">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>550</v>
       </c>
@@ -6175,8 +6436,11 @@
       <c r="K87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L87">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>556</v>
       </c>
@@ -6210,8 +6474,11 @@
       <c r="K88">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L88">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>562</v>
       </c>
@@ -6245,8 +6512,11 @@
       <c r="K89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L89">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>569</v>
       </c>
@@ -6280,8 +6550,11 @@
       <c r="K90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L90">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>574</v>
       </c>
@@ -6315,8 +6588,11 @@
       <c r="K91">
         <v>5</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L91">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>580</v>
       </c>
@@ -6350,8 +6626,11 @@
       <c r="K92">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L92">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>587</v>
       </c>
@@ -6385,8 +6664,11 @@
       <c r="K93">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L93">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>592</v>
       </c>
@@ -6420,8 +6702,11 @@
       <c r="K94">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L94">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>599</v>
       </c>
@@ -6455,8 +6740,11 @@
       <c r="K95">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L95">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>606</v>
       </c>
@@ -6490,8 +6778,11 @@
       <c r="K96">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L96">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>612</v>
       </c>
@@ -6525,8 +6816,11 @@
       <c r="K97">
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L97">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>619</v>
       </c>
@@ -6560,8 +6854,11 @@
       <c r="K98">
         <v>5</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L98">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>625</v>
       </c>
@@ -6595,8 +6892,11 @@
       <c r="K99">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L99">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>630</v>
       </c>
@@ -6630,8 +6930,11 @@
       <c r="K100">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L100">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>637</v>
       </c>
@@ -6665,8 +6968,11 @@
       <c r="K101">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L101">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>643</v>
       </c>
@@ -6700,8 +7006,11 @@
       <c r="K102">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L102">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>650</v>
       </c>
@@ -6735,8 +7044,11 @@
       <c r="K103">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L103">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>656</v>
       </c>
@@ -6770,8 +7082,11 @@
       <c r="K104">
         <v>5</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L104">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>662</v>
       </c>
@@ -6805,8 +7120,11 @@
       <c r="K105">
         <v>5</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L105">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>668</v>
       </c>
@@ -6840,8 +7158,11 @@
       <c r="K106">
         <v>5</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L106">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>673</v>
       </c>
@@ -6875,8 +7196,11 @@
       <c r="K107">
         <v>5</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L107">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>679</v>
       </c>
@@ -6910,8 +7234,11 @@
       <c r="K108">
         <v>5</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L108">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>686</v>
       </c>
@@ -6945,8 +7272,11 @@
       <c r="K109">
         <v>5</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L109">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>692</v>
       </c>
@@ -6980,8 +7310,11 @@
       <c r="K110">
         <v>5</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L110">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>699</v>
       </c>
@@ -7015,8 +7348,11 @@
       <c r="K111">
         <v>5</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L111">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>705</v>
       </c>
@@ -7050,8 +7386,11 @@
       <c r="K112">
         <v>5</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L112">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>711</v>
       </c>
@@ -7085,8 +7424,11 @@
       <c r="K113">
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L113">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>718</v>
       </c>
@@ -7120,8 +7462,11 @@
       <c r="K114">
         <v>5</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L114">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>724</v>
       </c>
@@ -7155,8 +7500,11 @@
       <c r="K115">
         <v>5</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L115">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>731</v>
       </c>
@@ -7190,8 +7538,11 @@
       <c r="K116">
         <v>5</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L116">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>738</v>
       </c>
@@ -7225,8 +7576,11 @@
       <c r="K117">
         <v>5</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L117">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>743</v>
       </c>
@@ -7260,8 +7614,11 @@
       <c r="K118">
         <v>5</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L118">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>750</v>
       </c>
@@ -7295,8 +7652,11 @@
       <c r="K119">
         <v>5</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L119">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>757</v>
       </c>
@@ -7330,8 +7690,11 @@
       <c r="K120">
         <v>5</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L120">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>764</v>
       </c>
@@ -7365,8 +7728,11 @@
       <c r="K121">
         <v>5</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L121">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>770</v>
       </c>
@@ -7400,8 +7766,11 @@
       <c r="K122">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L122">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>777</v>
       </c>
@@ -7435,8 +7804,11 @@
       <c r="K123">
         <v>5</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L123">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>783</v>
       </c>
@@ -7470,8 +7842,11 @@
       <c r="K124">
         <v>5</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L124">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>789</v>
       </c>
@@ -7505,8 +7880,11 @@
       <c r="K125">
         <v>5</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L125">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>796</v>
       </c>
@@ -7540,8 +7918,11 @@
       <c r="K126">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L126">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>801</v>
       </c>
@@ -7575,8 +7956,11 @@
       <c r="K127">
         <v>5</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L127">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>807</v>
       </c>
@@ -7610,8 +7994,11 @@
       <c r="K128">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L128">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>813</v>
       </c>
@@ -7645,8 +8032,11 @@
       <c r="K129">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L129">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>818</v>
       </c>
@@ -7680,8 +8070,11 @@
       <c r="K130">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L130">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>825</v>
       </c>
@@ -7715,8 +8108,11 @@
       <c r="K131">
         <v>5</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L131">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>832</v>
       </c>
@@ -7750,8 +8146,11 @@
       <c r="K132">
         <v>5</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L132">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>838</v>
       </c>
@@ -7785,8 +8184,11 @@
       <c r="K133">
         <v>5</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L133">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>843</v>
       </c>
@@ -7820,8 +8222,11 @@
       <c r="K134">
         <v>5</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L134">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>850</v>
       </c>
@@ -7855,8 +8260,11 @@
       <c r="K135">
         <v>5</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L135">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>855</v>
       </c>
@@ -7890,8 +8298,11 @@
       <c r="K136">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L136">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>861</v>
       </c>
@@ -7925,8 +8336,11 @@
       <c r="K137">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L137">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>867</v>
       </c>
@@ -7957,8 +8371,11 @@
       <c r="K138">
         <v>5</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L138">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>874</v>
       </c>
@@ -7992,8 +8409,11 @@
       <c r="K139">
         <v>5</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L139">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>881</v>
       </c>
@@ -8027,8 +8447,11 @@
       <c r="K140">
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L140">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>887</v>
       </c>
@@ -8062,8 +8485,11 @@
       <c r="K141">
         <v>5</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L141">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>893</v>
       </c>
@@ -8097,8 +8523,11 @@
       <c r="K142">
         <v>5</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L142">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>900</v>
       </c>
@@ -8132,8 +8561,11 @@
       <c r="K143">
         <v>5</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L143">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>905</v>
       </c>
@@ -8167,8 +8599,11 @@
       <c r="K144">
         <v>5</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L144">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>911</v>
       </c>
@@ -8202,8 +8637,11 @@
       <c r="K145">
         <v>5</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L145">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>916</v>
       </c>
@@ -8234,8 +8672,11 @@
       <c r="K146">
         <v>5</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L146">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>923</v>
       </c>
@@ -8265,6 +8706,9 @@
       </c>
       <c r="K147">
         <v>5</v>
+      </c>
+      <c r="L147">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>